<commit_message>
Removed category editing form from tours management
</commit_message>
<xml_diff>
--- a/tools/start-list.xlsx
+++ b/tools/start-list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artemk\Documents\RockComputer\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem\Documents\RockJudge\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9870" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="9870"/>
   </bookViews>
   <sheets>
     <sheet name="Clubs" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Formations" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
   <si>
     <t>Название клуба</t>
   </si>
@@ -96,7 +95,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -384,13 +383,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -405,15 +398,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -423,27 +416,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -737,19 +736,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="A2:C5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="68.1328125" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="14.65" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -776,16 +775,16 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="68.59765625" customWidth="1"/>
+    <col min="2" max="2" width="22.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="14.65" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -806,147 +805,147 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.59765625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" style="3" customWidth="1"/>
     <col min="3" max="3" width="7" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.73046875" style="3" customWidth="1"/>
     <col min="6" max="6" width="7" style="4" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="34.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="33.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="38.1328125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="28.86328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="34.1328125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="33.73046875" style="2" customWidth="1"/>
     <col min="11" max="11" width="4" style="3" customWidth="1"/>
-    <col min="12" max="12" width="33.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="33.73046875" style="2" customWidth="1"/>
     <col min="13" max="13" width="4" style="3" customWidth="1"/>
-    <col min="14" max="14" width="33.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="33.73046875" style="2" customWidth="1"/>
     <col min="15" max="15" width="4" style="3" customWidth="1"/>
-    <col min="16" max="16" width="33.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="33.73046875" style="2" customWidth="1"/>
     <col min="17" max="17" width="4" style="3" customWidth="1"/>
-    <col min="18" max="18" width="33.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="33.73046875" style="2" customWidth="1"/>
     <col min="19" max="19" width="4" style="4" customWidth="1"/>
-    <col min="20" max="20" width="33.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="33.73046875" style="2" customWidth="1"/>
     <col min="21" max="21" width="4" style="3" customWidth="1"/>
-    <col min="22" max="22" width="33.7109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="33.73046875" style="2" customWidth="1"/>
     <col min="23" max="23" width="4" style="4" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="3"/>
+    <col min="24" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="7" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:23" s="7" customFormat="1" ht="14.65" thickBot="1">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="18" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="26" t="s">
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="20"/>
-    </row>
-    <row r="2" spans="1:23" s="7" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="22"/>
+    </row>
+    <row r="2" spans="1:23" s="7" customFormat="1" ht="14.65" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="17" t="s">
+      <c r="P2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="11" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J1:W1"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="J1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -982,149 +981,149 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:BU15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F12" sqref="F12"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="30" customWidth="1"/>
-    <col min="2" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" style="4" customWidth="1"/>
-    <col min="6" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" style="4" customWidth="1"/>
-    <col min="10" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" style="4" customWidth="1"/>
-    <col min="14" max="15" width="21.7109375" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" customWidth="1"/>
-    <col min="17" max="17" width="5.140625" style="4" customWidth="1"/>
-    <col min="18" max="19" width="21.7109375" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" customWidth="1"/>
-    <col min="21" max="21" width="5.140625" style="4" customWidth="1"/>
-    <col min="22" max="23" width="21.7109375" customWidth="1"/>
-    <col min="24" max="24" width="8.5703125" customWidth="1"/>
-    <col min="25" max="25" width="5.140625" style="4" customWidth="1"/>
-    <col min="26" max="27" width="21.7109375" customWidth="1"/>
-    <col min="28" max="28" width="8.5703125" customWidth="1"/>
-    <col min="29" max="29" width="5.140625" style="4" customWidth="1"/>
-    <col min="30" max="31" width="21.7109375" customWidth="1"/>
-    <col min="32" max="32" width="8.5703125" customWidth="1"/>
-    <col min="33" max="33" width="5.140625" style="4" customWidth="1"/>
-    <col min="34" max="35" width="21.7109375" customWidth="1"/>
-    <col min="36" max="36" width="8.5703125" customWidth="1"/>
-    <col min="37" max="37" width="5.140625" style="4" customWidth="1"/>
-    <col min="38" max="39" width="21.7109375" customWidth="1"/>
-    <col min="40" max="40" width="8.5703125" customWidth="1"/>
-    <col min="41" max="41" width="5.140625" style="4" customWidth="1"/>
-    <col min="42" max="43" width="21.7109375" customWidth="1"/>
-    <col min="44" max="44" width="8.5703125" customWidth="1"/>
-    <col min="45" max="45" width="5.140625" style="4" customWidth="1"/>
-    <col min="46" max="47" width="21.7109375" customWidth="1"/>
-    <col min="48" max="48" width="8.5703125" customWidth="1"/>
-    <col min="49" max="49" width="5.140625" style="4" customWidth="1"/>
-    <col min="50" max="51" width="21.7109375" customWidth="1"/>
-    <col min="52" max="52" width="8.5703125" customWidth="1"/>
-    <col min="53" max="53" width="5.140625" style="4" customWidth="1"/>
-    <col min="54" max="55" width="21.7109375" customWidth="1"/>
-    <col min="56" max="56" width="8.5703125" customWidth="1"/>
-    <col min="57" max="57" width="5.140625" style="4" customWidth="1"/>
-    <col min="58" max="59" width="21.7109375" customWidth="1"/>
-    <col min="60" max="60" width="8.5703125" customWidth="1"/>
-    <col min="61" max="61" width="5.140625" style="4" customWidth="1"/>
-    <col min="62" max="63" width="21.7109375" customWidth="1"/>
-    <col min="64" max="64" width="8.5703125" customWidth="1"/>
-    <col min="65" max="65" width="5.140625" style="4" customWidth="1"/>
-    <col min="66" max="67" width="21.7109375" customWidth="1"/>
-    <col min="68" max="68" width="8.5703125" customWidth="1"/>
-    <col min="69" max="69" width="5.140625" style="4" customWidth="1"/>
-    <col min="70" max="71" width="21.7109375" customWidth="1"/>
-    <col min="72" max="72" width="8.5703125" customWidth="1"/>
-    <col min="73" max="73" width="5.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.1328125" style="16" customWidth="1"/>
+    <col min="2" max="3" width="21.73046875" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" customWidth="1"/>
+    <col min="5" max="5" width="5.1328125" style="4" customWidth="1"/>
+    <col min="6" max="7" width="21.73046875" customWidth="1"/>
+    <col min="8" max="8" width="8.59765625" customWidth="1"/>
+    <col min="9" max="9" width="5.1328125" style="4" customWidth="1"/>
+    <col min="10" max="11" width="21.73046875" customWidth="1"/>
+    <col min="12" max="12" width="8.59765625" customWidth="1"/>
+    <col min="13" max="13" width="5.1328125" style="4" customWidth="1"/>
+    <col min="14" max="15" width="21.73046875" customWidth="1"/>
+    <col min="16" max="16" width="8.59765625" customWidth="1"/>
+    <col min="17" max="17" width="5.1328125" style="4" customWidth="1"/>
+    <col min="18" max="19" width="21.73046875" customWidth="1"/>
+    <col min="20" max="20" width="8.59765625" customWidth="1"/>
+    <col min="21" max="21" width="5.1328125" style="4" customWidth="1"/>
+    <col min="22" max="23" width="21.73046875" customWidth="1"/>
+    <col min="24" max="24" width="8.59765625" customWidth="1"/>
+    <col min="25" max="25" width="5.1328125" style="4" customWidth="1"/>
+    <col min="26" max="27" width="21.73046875" customWidth="1"/>
+    <col min="28" max="28" width="8.59765625" customWidth="1"/>
+    <col min="29" max="29" width="5.1328125" style="4" customWidth="1"/>
+    <col min="30" max="31" width="21.73046875" customWidth="1"/>
+    <col min="32" max="32" width="8.59765625" customWidth="1"/>
+    <col min="33" max="33" width="5.1328125" style="4" customWidth="1"/>
+    <col min="34" max="35" width="21.73046875" customWidth="1"/>
+    <col min="36" max="36" width="8.59765625" customWidth="1"/>
+    <col min="37" max="37" width="5.1328125" style="4" customWidth="1"/>
+    <col min="38" max="39" width="21.73046875" customWidth="1"/>
+    <col min="40" max="40" width="8.59765625" customWidth="1"/>
+    <col min="41" max="41" width="5.1328125" style="4" customWidth="1"/>
+    <col min="42" max="43" width="21.73046875" customWidth="1"/>
+    <col min="44" max="44" width="8.59765625" customWidth="1"/>
+    <col min="45" max="45" width="5.1328125" style="4" customWidth="1"/>
+    <col min="46" max="47" width="21.73046875" customWidth="1"/>
+    <col min="48" max="48" width="8.59765625" customWidth="1"/>
+    <col min="49" max="49" width="5.1328125" style="4" customWidth="1"/>
+    <col min="50" max="51" width="21.73046875" customWidth="1"/>
+    <col min="52" max="52" width="8.59765625" customWidth="1"/>
+    <col min="53" max="53" width="5.1328125" style="4" customWidth="1"/>
+    <col min="54" max="55" width="21.73046875" customWidth="1"/>
+    <col min="56" max="56" width="8.59765625" customWidth="1"/>
+    <col min="57" max="57" width="5.1328125" style="4" customWidth="1"/>
+    <col min="58" max="59" width="21.73046875" customWidth="1"/>
+    <col min="60" max="60" width="8.59765625" customWidth="1"/>
+    <col min="61" max="61" width="5.1328125" style="4" customWidth="1"/>
+    <col min="62" max="63" width="21.73046875" customWidth="1"/>
+    <col min="64" max="64" width="8.59765625" customWidth="1"/>
+    <col min="65" max="65" width="5.1328125" style="4" customWidth="1"/>
+    <col min="66" max="67" width="21.73046875" customWidth="1"/>
+    <col min="68" max="68" width="8.59765625" customWidth="1"/>
+    <col min="69" max="69" width="5.1328125" style="4" customWidth="1"/>
+    <col min="70" max="71" width="21.73046875" customWidth="1"/>
+    <col min="72" max="72" width="8.59765625" customWidth="1"/>
+    <col min="73" max="73" width="5.1328125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="22"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="35"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="21"/>
-      <c r="AS1" s="22"/>
-      <c r="AT1" s="35"/>
-      <c r="AU1" s="21"/>
-      <c r="AV1" s="21"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="37"/>
-      <c r="BB1" s="35"/>
-      <c r="BC1" s="28"/>
-      <c r="BD1" s="28"/>
-      <c r="BE1" s="37"/>
-      <c r="BF1" s="35"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="28"/>
-      <c r="BI1" s="37"/>
-      <c r="BJ1" s="35"/>
-      <c r="BK1" s="28"/>
-      <c r="BL1" s="28"/>
-      <c r="BM1" s="37"/>
-      <c r="BN1" s="35"/>
-      <c r="BO1" s="28"/>
-      <c r="BP1" s="28"/>
-      <c r="BQ1" s="37"/>
-      <c r="BR1" s="35"/>
-      <c r="BS1" s="28"/>
-      <c r="BT1" s="28"/>
-      <c r="BU1" s="22"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="33"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="33"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="36"/>
+      <c r="AX1" s="33"/>
+      <c r="AY1" s="34"/>
+      <c r="AZ1" s="34"/>
+      <c r="BA1" s="35"/>
+      <c r="BB1" s="33"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="35"/>
+      <c r="BF1" s="33"/>
+      <c r="BG1" s="34"/>
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="35"/>
+      <c r="BJ1" s="33"/>
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BM1" s="35"/>
+      <c r="BN1" s="33"/>
+      <c r="BO1" s="34"/>
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="35"/>
+      <c r="BR1" s="33"/>
+      <c r="BS1" s="34"/>
+      <c r="BT1" s="34"/>
+      <c r="BU1" s="36"/>
     </row>
     <row r="2" spans="1:73">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="38"/>
@@ -1135,73 +1134,73 @@
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
       <c r="I2" s="40"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="35"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="35"/>
-      <c r="AQ2" s="21"/>
-      <c r="AR2" s="21"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="35"/>
-      <c r="AU2" s="21"/>
-      <c r="AV2" s="21"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="35"/>
-      <c r="AY2" s="28"/>
-      <c r="AZ2" s="28"/>
-      <c r="BA2" s="37"/>
-      <c r="BB2" s="35"/>
-      <c r="BC2" s="28"/>
-      <c r="BD2" s="28"/>
-      <c r="BE2" s="37"/>
-      <c r="BF2" s="35"/>
-      <c r="BG2" s="28"/>
-      <c r="BH2" s="28"/>
-      <c r="BI2" s="37"/>
-      <c r="BJ2" s="35"/>
-      <c r="BK2" s="28"/>
-      <c r="BL2" s="28"/>
-      <c r="BM2" s="37"/>
-      <c r="BN2" s="35"/>
-      <c r="BO2" s="28"/>
-      <c r="BP2" s="28"/>
-      <c r="BQ2" s="37"/>
-      <c r="BR2" s="35"/>
-      <c r="BS2" s="28"/>
-      <c r="BT2" s="28"/>
-      <c r="BU2" s="22"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="37"/>
+      <c r="AF2" s="37"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="37"/>
+      <c r="AJ2" s="37"/>
+      <c r="AK2" s="36"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="37"/>
+      <c r="AN2" s="37"/>
+      <c r="AO2" s="36"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="37"/>
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="36"/>
+      <c r="AT2" s="33"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="36"/>
+      <c r="AX2" s="33"/>
+      <c r="AY2" s="34"/>
+      <c r="AZ2" s="34"/>
+      <c r="BA2" s="35"/>
+      <c r="BB2" s="33"/>
+      <c r="BC2" s="34"/>
+      <c r="BD2" s="34"/>
+      <c r="BE2" s="35"/>
+      <c r="BF2" s="33"/>
+      <c r="BG2" s="34"/>
+      <c r="BH2" s="34"/>
+      <c r="BI2" s="35"/>
+      <c r="BJ2" s="33"/>
+      <c r="BK2" s="34"/>
+      <c r="BL2" s="34"/>
+      <c r="BM2" s="35"/>
+      <c r="BN2" s="33"/>
+      <c r="BO2" s="34"/>
+      <c r="BP2" s="34"/>
+      <c r="BQ2" s="35"/>
+      <c r="BR2" s="33"/>
+      <c r="BS2" s="34"/>
+      <c r="BT2" s="34"/>
+      <c r="BU2" s="36"/>
     </row>
     <row r="3" spans="1:73">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="38"/>
@@ -1212,156 +1211,164 @@
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
       <c r="I3" s="40"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="21"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="22"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="22"/>
-      <c r="AH3" s="35"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21"/>
-      <c r="AK3" s="22"/>
-      <c r="AL3" s="35"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="22"/>
-      <c r="AP3" s="35"/>
-      <c r="AQ3" s="21"/>
-      <c r="AR3" s="21"/>
-      <c r="AS3" s="22"/>
-      <c r="AT3" s="35"/>
-      <c r="AU3" s="21"/>
-      <c r="AV3" s="21"/>
-      <c r="AW3" s="22"/>
-      <c r="AX3" s="35"/>
-      <c r="AY3" s="28"/>
-      <c r="AZ3" s="28"/>
-      <c r="BA3" s="37"/>
-      <c r="BB3" s="35"/>
-      <c r="BC3" s="28"/>
-      <c r="BD3" s="28"/>
-      <c r="BE3" s="37"/>
-      <c r="BF3" s="35"/>
-      <c r="BG3" s="28"/>
-      <c r="BH3" s="28"/>
-      <c r="BI3" s="37"/>
-      <c r="BJ3" s="35"/>
-      <c r="BK3" s="28"/>
-      <c r="BL3" s="28"/>
-      <c r="BM3" s="37"/>
-      <c r="BN3" s="35"/>
-      <c r="BO3" s="28"/>
-      <c r="BP3" s="28"/>
-      <c r="BQ3" s="37"/>
-      <c r="BR3" s="35"/>
-      <c r="BS3" s="28"/>
-      <c r="BT3" s="28"/>
-      <c r="BU3" s="22"/>
-    </row>
-    <row r="4" spans="1:73" ht="15.75" thickBot="1">
-      <c r="A4" s="31" t="s">
+      <c r="J3" s="33"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="33"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="36"/>
+      <c r="AD3" s="33"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="36"/>
+      <c r="AH3" s="33"/>
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="36"/>
+      <c r="AL3" s="33"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AO3" s="36"/>
+      <c r="AP3" s="33"/>
+      <c r="AQ3" s="37"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="36"/>
+      <c r="AT3" s="33"/>
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
+      <c r="AW3" s="36"/>
+      <c r="AX3" s="33"/>
+      <c r="AY3" s="34"/>
+      <c r="AZ3" s="34"/>
+      <c r="BA3" s="35"/>
+      <c r="BB3" s="33"/>
+      <c r="BC3" s="34"/>
+      <c r="BD3" s="34"/>
+      <c r="BE3" s="35"/>
+      <c r="BF3" s="33"/>
+      <c r="BG3" s="34"/>
+      <c r="BH3" s="34"/>
+      <c r="BI3" s="35"/>
+      <c r="BJ3" s="33"/>
+      <c r="BK3" s="34"/>
+      <c r="BL3" s="34"/>
+      <c r="BM3" s="35"/>
+      <c r="BN3" s="33"/>
+      <c r="BO3" s="34"/>
+      <c r="BP3" s="34"/>
+      <c r="BQ3" s="35"/>
+      <c r="BR3" s="33"/>
+      <c r="BS3" s="34"/>
+      <c r="BT3" s="34"/>
+      <c r="BU3" s="36"/>
+    </row>
+    <row r="4" spans="1:73" ht="14.65" thickBot="1">
+      <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="23"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="23"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="23"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="23"/>
-      <c r="AF4" s="23"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="33"/>
-      <c r="AI4" s="23"/>
-      <c r="AJ4" s="23"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="33"/>
-      <c r="AM4" s="23"/>
-      <c r="AN4" s="23"/>
-      <c r="AO4" s="24"/>
-      <c r="AP4" s="33"/>
-      <c r="AQ4" s="23"/>
-      <c r="AR4" s="23"/>
-      <c r="AS4" s="24"/>
-      <c r="AT4" s="33"/>
-      <c r="AU4" s="23"/>
-      <c r="AV4" s="23"/>
-      <c r="AW4" s="24"/>
-      <c r="AX4" s="33"/>
-      <c r="AY4" s="23"/>
-      <c r="AZ4" s="23"/>
-      <c r="BA4" s="36"/>
-      <c r="BB4" s="33"/>
-      <c r="BC4" s="23"/>
-      <c r="BD4" s="23"/>
-      <c r="BE4" s="36"/>
-      <c r="BF4" s="33"/>
-      <c r="BG4" s="23"/>
-      <c r="BH4" s="23"/>
-      <c r="BI4" s="36"/>
-      <c r="BJ4" s="33"/>
-      <c r="BK4" s="23"/>
-      <c r="BL4" s="23"/>
-      <c r="BM4" s="36"/>
-      <c r="BN4" s="33"/>
-      <c r="BO4" s="23"/>
-      <c r="BP4" s="23"/>
-      <c r="BQ4" s="36"/>
-      <c r="BR4" s="33"/>
-      <c r="BS4" s="23"/>
-      <c r="BT4" s="23"/>
-      <c r="BU4" s="24"/>
-    </row>
-    <row r="5" spans="1:73" ht="15.75" thickBot="1">
-      <c r="A5" s="32" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="32"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="32"/>
+      <c r="AH4" s="29"/>
+      <c r="AI4" s="30"/>
+      <c r="AJ4" s="30"/>
+      <c r="AK4" s="32"/>
+      <c r="AL4" s="29"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="30"/>
+      <c r="AO4" s="32"/>
+      <c r="AP4" s="29"/>
+      <c r="AQ4" s="30"/>
+      <c r="AR4" s="30"/>
+      <c r="AS4" s="32"/>
+      <c r="AT4" s="29"/>
+      <c r="AU4" s="30"/>
+      <c r="AV4" s="30"/>
+      <c r="AW4" s="32"/>
+      <c r="AX4" s="29"/>
+      <c r="AY4" s="30"/>
+      <c r="AZ4" s="30"/>
+      <c r="BA4" s="31"/>
+      <c r="BB4" s="29"/>
+      <c r="BC4" s="30"/>
+      <c r="BD4" s="30"/>
+      <c r="BE4" s="31"/>
+      <c r="BF4" s="29"/>
+      <c r="BG4" s="30"/>
+      <c r="BH4" s="30"/>
+      <c r="BI4" s="31"/>
+      <c r="BJ4" s="29"/>
+      <c r="BK4" s="30"/>
+      <c r="BL4" s="30"/>
+      <c r="BM4" s="31"/>
+      <c r="BN4" s="29"/>
+      <c r="BO4" s="30"/>
+      <c r="BP4" s="30"/>
+      <c r="BQ4" s="31"/>
+      <c r="BR4" s="29"/>
+      <c r="BS4" s="30"/>
+      <c r="BT4" s="30"/>
+      <c r="BU4" s="32"/>
+    </row>
+    <row r="5" spans="1:73" ht="14.65" thickBot="1">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="6"/>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1568,78 +1575,91 @@
       </c>
     </row>
     <row r="6" spans="1:73">
-      <c r="E6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="Q6" s="34"/>
-      <c r="U6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="AC6" s="34"/>
-      <c r="AG6" s="34"/>
-      <c r="AK6" s="34"/>
-      <c r="AO6" s="34"/>
-      <c r="AS6" s="34"/>
-      <c r="AW6" s="34"/>
-      <c r="BA6" s="34"/>
-      <c r="BE6" s="34"/>
-      <c r="BI6" s="34"/>
-      <c r="BM6" s="34"/>
-      <c r="BQ6" s="34"/>
-      <c r="BU6" s="34"/>
+      <c r="E6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AG6" s="19"/>
+      <c r="AK6" s="19"/>
+      <c r="AO6" s="19"/>
+      <c r="AS6" s="19"/>
+      <c r="AW6" s="19"/>
+      <c r="BA6" s="19"/>
+      <c r="BE6" s="19"/>
+      <c r="BI6" s="19"/>
+      <c r="BM6" s="19"/>
+      <c r="BQ6" s="19"/>
+      <c r="BU6" s="19"/>
     </row>
     <row r="7" spans="1:73">
-      <c r="E7" s="34"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:73">
-      <c r="E8" s="34"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:73">
-      <c r="E9" s="34"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:73">
-      <c r="E10" s="34"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:73">
-      <c r="E11" s="34"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:73">
-      <c r="E12" s="34"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:73">
-      <c r="E13" s="34"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:73">
-      <c r="E14" s="34"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:73">
-      <c r="E15" s="34"/>
+      <c r="E15" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="AX4:BA4"/>
-    <mergeCell ref="BB4:BE4"/>
-    <mergeCell ref="BF4:BI4"/>
-    <mergeCell ref="BJ4:BM4"/>
-    <mergeCell ref="BN4:BQ4"/>
-    <mergeCell ref="BR4:BU4"/>
-    <mergeCell ref="AX3:BA3"/>
-    <mergeCell ref="BB3:BE3"/>
-    <mergeCell ref="BF3:BI3"/>
-    <mergeCell ref="BJ3:BM3"/>
-    <mergeCell ref="BN3:BQ3"/>
-    <mergeCell ref="BR3:BU3"/>
-    <mergeCell ref="AX2:BA2"/>
-    <mergeCell ref="BB2:BE2"/>
-    <mergeCell ref="BF2:BI2"/>
-    <mergeCell ref="BJ2:BM2"/>
-    <mergeCell ref="BN2:BQ2"/>
-    <mergeCell ref="BR2:BU2"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="AT2:AW2"/>
+    <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AH3:AK3"/>
     <mergeCell ref="AL3:AO3"/>
     <mergeCell ref="AP3:AS3"/>
@@ -1650,44 +1670,31 @@
     <mergeCell ref="AL4:AO4"/>
     <mergeCell ref="AP4:AS4"/>
     <mergeCell ref="AT4:AW4"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="AL2:AO2"/>
-    <mergeCell ref="AP2:AS2"/>
-    <mergeCell ref="AT2:AW2"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="Z3:AC3"/>
     <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="BR2:BU2"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="AX2:BA2"/>
+    <mergeCell ref="BB2:BE2"/>
+    <mergeCell ref="BF2:BI2"/>
+    <mergeCell ref="BJ2:BM2"/>
+    <mergeCell ref="BN2:BQ2"/>
+    <mergeCell ref="BR4:BU4"/>
+    <mergeCell ref="AX3:BA3"/>
+    <mergeCell ref="BB3:BE3"/>
+    <mergeCell ref="BF3:BI3"/>
+    <mergeCell ref="BJ3:BM3"/>
+    <mergeCell ref="BN3:BQ3"/>
+    <mergeCell ref="BR3:BU3"/>
+    <mergeCell ref="AX4:BA4"/>
+    <mergeCell ref="BB4:BE4"/>
+    <mergeCell ref="BF4:BI4"/>
+    <mergeCell ref="BJ4:BM4"/>
+    <mergeCell ref="BN4:BQ4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I199 M6:M199 Q6:Q199 U6:U199 Y6:Y199 AC6:AC199 AG6:AG199 AK6:AK199 AO6:AO199 AS6:AS199 AW6:AW199 BA6:BA199 BE6:BE199 BI6:BI199 BM6:BM199 BQ6:BQ199 E6:E199 BU6:BU199">
@@ -1709,7 +1716,7 @@
           <x14:formula1>
             <xm:f>Clubs!$A$2:$A$100</xm:f>
           </x14:formula1>
-          <xm:sqref>BR3:BU3 B3 J3:M3 N3:Q3 R3:U3 V3:Y3 Z3:AC3 AD3:AG3 AH3:AK3 AL3:AO3 AP3:AS3 AT3:AW3 AX3:BA3 BB3:BE3 BF3:BI3 BJ3:BM3 BN3:BQ3 F3</xm:sqref>
+          <xm:sqref>B3 J3:BU3 F3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Resolved #39, #108: Added discipline judges
</commit_message>
<xml_diff>
--- a/tools/start-list.xlsx
+++ b/tools/start-list.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21930" windowHeight="10650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="5060" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Disciplines" sheetId="2" r:id="rId1"/>
     <sheet name="Judges" sheetId="3" r:id="rId2"/>
-    <sheet name="Clubs" sheetId="1" r:id="rId3"/>
-    <sheet name="Couples, solo" sheetId="4" r:id="rId4"/>
-    <sheet name="Formations" sheetId="5" r:id="rId5"/>
+    <sheet name="Discipline judges" sheetId="6" r:id="rId3"/>
+    <sheet name="Clubs" sheetId="1" r:id="rId4"/>
+    <sheet name="Couples, solo" sheetId="4" r:id="rId5"/>
+    <sheet name="Formations" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>Название клуба</t>
   </si>
@@ -116,6 +117,9 @@
   </si>
   <si>
     <t>Акро 5 - описание</t>
+  </si>
+  <si>
+    <t>Судья</t>
   </si>
 </sst>
 </file>
@@ -708,7 +712,7 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -788,12 +792,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J144"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -807,12 +812,10 @@
     <col min="3" max="3" width="8.7265625" style="29"/>
     <col min="4" max="4" width="35.54296875" customWidth="1"/>
     <col min="5" max="5" width="11.81640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-    <col min="9" max="9" width="29.90625" style="11" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" style="11" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="29.90625" style="11" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="14" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:8" s="14" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -828,877 +831,148 @@
       <c r="E1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="D3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="D4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
-    <row r="5" spans="1:10">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="D5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="22"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="22"/>
-      <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:10">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:10">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="D11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:10">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="D12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:10" s="22" customFormat="1">
+    </row>
+    <row r="13" spans="1:8" s="22" customFormat="1">
       <c r="C13" s="29"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" s="22" customFormat="1">
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" s="22" customFormat="1">
       <c r="C14" s="29"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:10">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="D16" s="12"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="F23" s="12"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="F24" s="12"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="F25" s="12"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="F28" s="12"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="F32" s="12"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="F34" s="12"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="F35" s="12"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="F36" s="12"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="F37" s="12"/>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="F38" s="12"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="F39" s="12"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="F40" s="12"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="F41" s="12"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="F42" s="12"/>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="F43" s="12"/>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="F44" s="12"/>
-    </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="F46" s="12"/>
-    </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="F47" s="12"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="F48" s="12"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="F49" s="12"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="F50" s="12"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="F51" s="12"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="F53" s="12"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="F54" s="12"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="F55" s="12"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="F56" s="12"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="F57" s="12"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="F58" s="12"/>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="F59" s="12"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="F60" s="12"/>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="F61" s="12"/>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="12"/>
-      <c r="B62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="F62" s="12"/>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="F63" s="12"/>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="F64" s="12"/>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="F65" s="12"/>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="F66" s="12"/>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="F67" s="12"/>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="F68" s="12"/>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="F69" s="12"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="F70" s="12"/>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="F71" s="12"/>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="F72" s="12"/>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="F73" s="12"/>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
-      <c r="D74" s="12"/>
-      <c r="F74" s="12"/>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="F75" s="12"/>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="F76" s="12"/>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="F77" s="12"/>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="F78" s="12"/>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="F79" s="12"/>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="F80" s="12"/>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="F81" s="12"/>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="F82" s="12"/>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="F83" s="12"/>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="F84" s="12"/>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="12"/>
-      <c r="B85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="F85" s="12"/>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="F86" s="12"/>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="F87" s="12"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="F88" s="12"/>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
-      <c r="D89" s="12"/>
-      <c r="F89" s="12"/>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
-      <c r="D90" s="12"/>
-      <c r="F90" s="12"/>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="12"/>
-      <c r="B91" s="12"/>
-      <c r="D91" s="12"/>
-      <c r="F91" s="12"/>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="12"/>
-      <c r="B92" s="12"/>
-      <c r="D92" s="12"/>
-      <c r="F92" s="12"/>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
-      <c r="D93" s="12"/>
-      <c r="F93" s="12"/>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
-      <c r="D94" s="12"/>
-      <c r="F94" s="12"/>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="12"/>
-      <c r="B95" s="12"/>
-      <c r="D95" s="12"/>
-      <c r="F95" s="12"/>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
-      <c r="D96" s="12"/>
-      <c r="F96" s="12"/>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
-      <c r="D97" s="12"/>
-      <c r="F97" s="12"/>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="F98" s="12"/>
-    </row>
-    <row r="99" spans="1:6">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="F99" s="12"/>
-    </row>
-    <row r="100" spans="1:6">
-      <c r="A100" s="12"/>
-      <c r="B100" s="12"/>
-      <c r="D100" s="12"/>
-      <c r="F100" s="12"/>
-    </row>
-    <row r="101" spans="1:6">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="F101" s="12"/>
-    </row>
-    <row r="102" spans="1:6">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="F102" s="12"/>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
-      <c r="D103" s="12"/>
-      <c r="F103" s="12"/>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
-      <c r="D104" s="12"/>
-      <c r="F104" s="12"/>
-    </row>
-    <row r="105" spans="1:6">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
-      <c r="D105" s="12"/>
-      <c r="F105" s="12"/>
-    </row>
-    <row r="106" spans="1:6">
-      <c r="A106" s="12"/>
-      <c r="B106" s="12"/>
-      <c r="D106" s="12"/>
-      <c r="F106" s="12"/>
-    </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="12"/>
-      <c r="B107" s="12"/>
-      <c r="D107" s="12"/>
-      <c r="F107" s="12"/>
-    </row>
-    <row r="108" spans="1:6">
-      <c r="A108" s="12"/>
-      <c r="B108" s="12"/>
-      <c r="D108" s="12"/>
-      <c r="F108" s="12"/>
-    </row>
-    <row r="109" spans="1:6">
-      <c r="A109" s="12"/>
-      <c r="B109" s="12"/>
-      <c r="D109" s="12"/>
-      <c r="F109" s="12"/>
-    </row>
-    <row r="110" spans="1:6">
-      <c r="A110" s="12"/>
-      <c r="B110" s="12"/>
-      <c r="D110" s="12"/>
-      <c r="F110" s="12"/>
-    </row>
-    <row r="111" spans="1:6">
-      <c r="A111" s="12"/>
-      <c r="B111" s="12"/>
-      <c r="D111" s="12"/>
-      <c r="F111" s="12"/>
-    </row>
-    <row r="112" spans="1:6">
-      <c r="A112" s="12"/>
-      <c r="B112" s="12"/>
-      <c r="D112" s="12"/>
-      <c r="F112" s="12"/>
-    </row>
-    <row r="113" spans="1:6">
-      <c r="A113" s="12"/>
-      <c r="B113" s="12"/>
-      <c r="D113" s="12"/>
-      <c r="F113" s="12"/>
-    </row>
-    <row r="114" spans="1:6">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
-      <c r="D114" s="12"/>
-      <c r="F114" s="12"/>
-    </row>
-    <row r="115" spans="1:6">
-      <c r="A115" s="12"/>
-      <c r="B115" s="12"/>
-      <c r="D115" s="12"/>
-      <c r="F115" s="12"/>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116" s="12"/>
-      <c r="B116" s="12"/>
-      <c r="D116" s="12"/>
-      <c r="F116" s="12"/>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" s="12"/>
-      <c r="B117" s="12"/>
-      <c r="D117" s="12"/>
-      <c r="F117" s="12"/>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" s="12"/>
-      <c r="B118" s="12"/>
-      <c r="D118" s="12"/>
-      <c r="F118" s="12"/>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
-      <c r="D119" s="12"/>
-      <c r="F119" s="12"/>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
-      <c r="D120" s="12"/>
-      <c r="F120" s="12"/>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" s="12"/>
-      <c r="B121" s="12"/>
-      <c r="D121" s="12"/>
-      <c r="F121" s="12"/>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
-      <c r="D122" s="12"/>
-      <c r="F122" s="12"/>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" s="12"/>
-      <c r="B123" s="12"/>
-      <c r="D123" s="12"/>
-      <c r="F123" s="12"/>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="12"/>
-      <c r="B124" s="12"/>
-      <c r="D124" s="12"/>
-      <c r="F124" s="12"/>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
-      <c r="D125" s="12"/>
-      <c r="F125" s="12"/>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="12"/>
-      <c r="B126" s="12"/>
-      <c r="D126" s="12"/>
-      <c r="F126" s="12"/>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="12"/>
-      <c r="B127" s="12"/>
-      <c r="D127" s="12"/>
-      <c r="F127" s="12"/>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" s="12"/>
-      <c r="B128" s="12"/>
-      <c r="D128" s="12"/>
-      <c r="F128" s="12"/>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" s="12"/>
-      <c r="B129" s="12"/>
-      <c r="D129" s="12"/>
-      <c r="F129" s="12"/>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" s="12"/>
-      <c r="B130" s="12"/>
-      <c r="D130" s="12"/>
-      <c r="F130" s="12"/>
-    </row>
-    <row r="131" spans="1:6">
-      <c r="A131" s="12"/>
-      <c r="B131" s="12"/>
-      <c r="D131" s="12"/>
-      <c r="F131" s="12"/>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" s="12"/>
-      <c r="B132" s="12"/>
-      <c r="D132" s="12"/>
-      <c r="F132" s="12"/>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" s="12"/>
-      <c r="B133" s="12"/>
-      <c r="D133" s="12"/>
-      <c r="F133" s="12"/>
-    </row>
-    <row r="134" spans="1:6">
-      <c r="A134" s="12"/>
-      <c r="B134" s="12"/>
-      <c r="D134" s="12"/>
-      <c r="F134" s="12"/>
-    </row>
-    <row r="135" spans="1:6">
-      <c r="A135" s="12"/>
-      <c r="B135" s="12"/>
-      <c r="D135" s="12"/>
-      <c r="F135" s="12"/>
-    </row>
-    <row r="136" spans="1:6">
-      <c r="A136" s="12"/>
-      <c r="B136" s="12"/>
-      <c r="D136" s="12"/>
-      <c r="F136" s="12"/>
-    </row>
-    <row r="137" spans="1:6">
-      <c r="A137" s="12"/>
-      <c r="B137" s="12"/>
-      <c r="D137" s="12"/>
-      <c r="F137" s="12"/>
-    </row>
-    <row r="138" spans="1:6">
-      <c r="A138" s="12"/>
-      <c r="B138" s="12"/>
-      <c r="D138" s="12"/>
-      <c r="F138" s="12"/>
-    </row>
-    <row r="139" spans="1:6">
-      <c r="A139" s="12"/>
-      <c r="B139" s="12"/>
-      <c r="D139" s="12"/>
-      <c r="F139" s="12"/>
-    </row>
-    <row r="140" spans="1:6">
-      <c r="A140" s="12"/>
-      <c r="B140" s="12"/>
-      <c r="D140" s="12"/>
-      <c r="F140" s="12"/>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" s="12"/>
-      <c r="B141" s="12"/>
-      <c r="D141" s="12"/>
-      <c r="F141" s="12"/>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="A142" s="12"/>
-      <c r="B142" s="12"/>
-      <c r="D142" s="12"/>
-      <c r="F142" s="12"/>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" s="12"/>
-      <c r="B143" s="12"/>
-      <c r="D143" s="12"/>
-      <c r="F143" s="12"/>
-    </row>
-    <row r="144" spans="1:6">
-      <c r="A144" s="12"/>
-      <c r="B144" s="12"/>
-      <c r="D144" s="12"/>
-      <c r="F144" s="12"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F144">
-      <formula1>$J$2:$J$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B144">
-      <formula1>$I$2:$I$9</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B2:B16">
+      <formula1>$H$2:$H$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="47.90625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="36.6328125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" style="22" customWidth="1"/>
+    <col min="4" max="9" width="8.7265625" style="22"/>
+    <col min="10" max="10" width="11.453125" style="11" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="14" customFormat="1" ht="15" thickBot="1">
+      <c r="A1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9 C11:C144">
+      <formula1>$J$2:$J$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Disciplines!$B$2:$B$200</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A9 A11:A500</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Judges!$D$2:$D$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2 B11 B19:B20 B28:B29 B37:B500</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1760,7 +1034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1374"/>
   <sheetViews>
@@ -7543,11 +6817,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>

</xml_diff>

<commit_message>
Updated xlsx parsing script to work with multiple programs
</commit_message>
<xml_diff>
--- a/tools/start-list.xlsx
+++ b/tools/start-list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="5060" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9870" windowHeight="5060"/>
   </bookViews>
   <sheets>
     <sheet name="Disciplines" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Название клуба</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Судья</t>
+  </si>
+  <si>
+    <t>Программа</t>
+  </si>
+  <si>
+    <t>Исп. для</t>
   </si>
 </sst>
 </file>
@@ -351,7 +357,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -390,6 +396,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -712,7 +721,7 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -1036,7 +1045,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1374"/>
+  <dimension ref="A1:V1374"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
@@ -1057,8 +1066,8 @@
     <col min="8" max="8" width="38.1796875" style="4" customWidth="1"/>
     <col min="9" max="9" width="28.81640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="34.1796875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="33.7265625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.7265625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.1796875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="11" style="24" customWidth="1"/>
     <col min="13" max="13" width="33.7265625" style="2" customWidth="1"/>
     <col min="14" max="14" width="5.7265625" style="1" customWidth="1"/>
     <col min="15" max="15" width="33.7265625" style="2" customWidth="1"/>
@@ -1066,48 +1075,54 @@
     <col min="17" max="17" width="33.7265625" style="2" customWidth="1"/>
     <col min="18" max="18" width="5.7265625" style="1" customWidth="1"/>
     <col min="19" max="19" width="33.7265625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="5.7265625" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="1"/>
+    <col min="20" max="20" width="5.7265625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="33.7265625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="5.7265625" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="15" customFormat="1" ht="15" thickBot="1">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:22" s="15" customFormat="1" ht="15" thickBot="1">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="32" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="30" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="35"/>
+      <c r="M1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
       <c r="T1" s="34"/>
-    </row>
-    <row r="2" spans="1:20" s="15" customFormat="1" ht="15" thickBot="1">
-      <c r="A2" s="31"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="35"/>
+    </row>
+    <row r="2" spans="1:22" s="15" customFormat="1" ht="15" thickBot="1">
+      <c r="A2" s="32"/>
       <c r="B2" s="18" t="s">
         <v>15</v>
       </c>
@@ -1126,41 +1141,47 @@
       <c r="G2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="18" t="s">
-        <v>27</v>
+      <c r="H2" s="32"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="30" t="s">
+        <v>20</v>
       </c>
-      <c r="L2" s="19" t="s">
-        <v>18</v>
+      <c r="L2" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R2" s="19" t="s">
         <v>18</v>
       </c>
       <c r="S2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="V2" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:22">
       <c r="B3" s="23"/>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
@@ -1170,8 +1191,8 @@
       <c r="H3" s="26"/>
       <c r="I3" s="24"/>
       <c r="J3" s="25"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="23"/>
       <c r="N3" s="24"/>
       <c r="O3" s="23"/>
@@ -1179,9 +1200,11 @@
       <c r="Q3" s="23"/>
       <c r="R3" s="24"/>
       <c r="S3" s="23"/>
-      <c r="T3" s="25"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="T3" s="24"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="25"/>
+    </row>
+    <row r="4" spans="1:22">
       <c r="B4" s="23"/>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
@@ -1191,8 +1214,8 @@
       <c r="H4" s="26"/>
       <c r="I4" s="24"/>
       <c r="J4" s="25"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
       <c r="M4" s="23"/>
       <c r="N4" s="24"/>
       <c r="O4" s="23"/>
@@ -1200,9 +1223,11 @@
       <c r="Q4" s="23"/>
       <c r="R4" s="24"/>
       <c r="S4" s="23"/>
-      <c r="T4" s="25"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="T4" s="24"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="25"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="7"/>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
@@ -1213,8 +1238,8 @@
       <c r="H5" s="26"/>
       <c r="I5" s="24"/>
       <c r="J5" s="25"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
       <c r="M5" s="23"/>
       <c r="N5" s="24"/>
       <c r="O5" s="23"/>
@@ -1222,9 +1247,11 @@
       <c r="Q5" s="23"/>
       <c r="R5" s="24"/>
       <c r="S5" s="23"/>
-      <c r="T5" s="25"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="T5" s="24"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="25"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="7"/>
       <c r="B6" s="23"/>
       <c r="C6" s="28"/>
@@ -1235,18 +1262,20 @@
       <c r="H6" s="26"/>
       <c r="I6" s="24"/>
       <c r="J6" s="25"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
       <c r="M6" s="23"/>
-      <c r="N6" s="28"/>
+      <c r="N6" s="24"/>
       <c r="O6" s="23"/>
       <c r="P6" s="28"/>
       <c r="Q6" s="23"/>
       <c r="R6" s="28"/>
       <c r="S6" s="23"/>
-      <c r="T6" s="25"/>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="T6" s="28"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="25"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="7"/>
       <c r="B7" s="23"/>
       <c r="C7" s="28"/>
@@ -1257,18 +1286,20 @@
       <c r="H7" s="26"/>
       <c r="I7" s="24"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
       <c r="M7" s="23"/>
-      <c r="N7" s="28"/>
+      <c r="N7" s="24"/>
       <c r="O7" s="23"/>
       <c r="P7" s="28"/>
       <c r="Q7" s="23"/>
       <c r="R7" s="28"/>
       <c r="S7" s="23"/>
-      <c r="T7" s="25"/>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="T7" s="28"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="25"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="7"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24"/>
@@ -1279,7 +1310,7 @@
       <c r="H8" s="26"/>
       <c r="I8" s="24"/>
       <c r="J8" s="25"/>
-      <c r="K8" s="23"/>
+      <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="23"/>
       <c r="N8" s="28"/>
@@ -1288,9 +1319,11 @@
       <c r="Q8" s="23"/>
       <c r="R8" s="28"/>
       <c r="S8" s="23"/>
-      <c r="T8" s="25"/>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="T8" s="28"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="25"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="7"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
@@ -1301,8 +1334,6 @@
       <c r="H9" s="26"/>
       <c r="I9" s="24"/>
       <c r="J9" s="25"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
       <c r="M9" s="23"/>
       <c r="N9" s="24"/>
       <c r="O9" s="23"/>
@@ -1310,9 +1341,11 @@
       <c r="Q9" s="23"/>
       <c r="R9" s="24"/>
       <c r="S9" s="23"/>
-      <c r="T9" s="25"/>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="T9" s="24"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="25"/>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="7"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
@@ -1323,8 +1356,6 @@
       <c r="H10" s="26"/>
       <c r="I10" s="24"/>
       <c r="J10" s="25"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
       <c r="M10" s="23"/>
       <c r="N10" s="24"/>
       <c r="O10" s="23"/>
@@ -1332,9 +1363,11 @@
       <c r="Q10" s="23"/>
       <c r="R10" s="24"/>
       <c r="S10" s="23"/>
-      <c r="T10" s="25"/>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="T10" s="24"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="25"/>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="7"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
@@ -1345,8 +1378,6 @@
       <c r="H11" s="26"/>
       <c r="I11" s="24"/>
       <c r="J11" s="25"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
       <c r="M11" s="23"/>
       <c r="N11" s="24"/>
       <c r="O11" s="23"/>
@@ -1354,9 +1385,11 @@
       <c r="Q11" s="23"/>
       <c r="R11" s="24"/>
       <c r="S11" s="23"/>
-      <c r="T11" s="25"/>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="T11" s="24"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="25"/>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="7"/>
       <c r="B12" s="23"/>
       <c r="C12" s="28"/>
@@ -1367,8 +1400,6 @@
       <c r="H12" s="26"/>
       <c r="I12" s="24"/>
       <c r="J12" s="25"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
       <c r="M12" s="23"/>
       <c r="N12" s="24"/>
       <c r="O12" s="23"/>
@@ -1376,9 +1407,11 @@
       <c r="Q12" s="23"/>
       <c r="R12" s="24"/>
       <c r="S12" s="23"/>
-      <c r="T12" s="25"/>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="T12" s="24"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="25"/>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="7"/>
       <c r="B13" s="23"/>
       <c r="C13" s="28"/>
@@ -1389,8 +1422,6 @@
       <c r="H13" s="26"/>
       <c r="I13" s="24"/>
       <c r="J13" s="25"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
       <c r="M13" s="23"/>
       <c r="N13" s="24"/>
       <c r="O13" s="23"/>
@@ -1398,9 +1429,11 @@
       <c r="Q13" s="23"/>
       <c r="R13" s="24"/>
       <c r="S13" s="23"/>
-      <c r="T13" s="25"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="T13" s="24"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="25"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="7"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -1411,8 +1444,6 @@
       <c r="H14" s="26"/>
       <c r="I14" s="24"/>
       <c r="J14" s="25"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
       <c r="M14" s="23"/>
       <c r="N14" s="24"/>
       <c r="O14" s="23"/>
@@ -1420,9 +1451,11 @@
       <c r="Q14" s="23"/>
       <c r="R14" s="24"/>
       <c r="S14" s="23"/>
-      <c r="T14" s="25"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="T14" s="24"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="25"/>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="7"/>
       <c r="B15" s="23"/>
       <c r="C15" s="28"/>
@@ -1433,8 +1466,6 @@
       <c r="H15" s="26"/>
       <c r="I15" s="24"/>
       <c r="J15" s="25"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
       <c r="M15" s="23"/>
       <c r="N15" s="24"/>
       <c r="O15" s="23"/>
@@ -1442,9 +1473,11 @@
       <c r="Q15" s="23"/>
       <c r="R15" s="24"/>
       <c r="S15" s="23"/>
-      <c r="T15" s="25"/>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="T15" s="24"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="25"/>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="7"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
@@ -1455,8 +1488,6 @@
       <c r="H16" s="26"/>
       <c r="I16" s="24"/>
       <c r="J16" s="25"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
       <c r="M16" s="23"/>
       <c r="N16" s="24"/>
       <c r="O16" s="23"/>
@@ -1464,9 +1495,11 @@
       <c r="Q16" s="23"/>
       <c r="R16" s="24"/>
       <c r="S16" s="23"/>
-      <c r="T16" s="25"/>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="T16" s="24"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="25"/>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="7"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24"/>
@@ -1477,8 +1510,6 @@
       <c r="H17" s="26"/>
       <c r="I17" s="24"/>
       <c r="J17" s="25"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
       <c r="M17" s="23"/>
       <c r="N17" s="24"/>
       <c r="O17" s="23"/>
@@ -1486,9 +1517,11 @@
       <c r="Q17" s="23"/>
       <c r="R17" s="24"/>
       <c r="S17" s="23"/>
-      <c r="T17" s="25"/>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="T17" s="24"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="25"/>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="7"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24"/>
@@ -1499,8 +1532,6 @@
       <c r="H18" s="26"/>
       <c r="I18" s="24"/>
       <c r="J18" s="25"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
       <c r="M18" s="23"/>
       <c r="N18" s="24"/>
       <c r="O18" s="23"/>
@@ -1508,9 +1539,11 @@
       <c r="Q18" s="23"/>
       <c r="R18" s="24"/>
       <c r="S18" s="23"/>
-      <c r="T18" s="25"/>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="T18" s="24"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="25"/>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="7"/>
       <c r="B19" s="23"/>
       <c r="C19" s="28"/>
@@ -1521,8 +1554,6 @@
       <c r="H19" s="26"/>
       <c r="I19" s="24"/>
       <c r="J19" s="25"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
       <c r="M19" s="23"/>
       <c r="N19" s="24"/>
       <c r="O19" s="23"/>
@@ -1530,9 +1561,11 @@
       <c r="Q19" s="23"/>
       <c r="R19" s="24"/>
       <c r="S19" s="23"/>
-      <c r="T19" s="25"/>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="T19" s="24"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="25"/>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="7"/>
       <c r="B20" s="23"/>
       <c r="C20" s="28"/>
@@ -1543,8 +1576,6 @@
       <c r="H20" s="26"/>
       <c r="I20" s="24"/>
       <c r="J20" s="25"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
       <c r="M20" s="23"/>
       <c r="N20" s="24"/>
       <c r="O20" s="23"/>
@@ -1552,9 +1583,11 @@
       <c r="Q20" s="23"/>
       <c r="R20" s="24"/>
       <c r="S20" s="23"/>
-      <c r="T20" s="25"/>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="T20" s="24"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="25"/>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="7"/>
       <c r="B21" s="23"/>
       <c r="C21" s="28"/>
@@ -1565,8 +1598,6 @@
       <c r="H21" s="26"/>
       <c r="I21" s="24"/>
       <c r="J21" s="25"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
       <c r="M21" s="23"/>
       <c r="N21" s="24"/>
       <c r="O21" s="23"/>
@@ -1574,9 +1605,11 @@
       <c r="Q21" s="23"/>
       <c r="R21" s="24"/>
       <c r="S21" s="23"/>
-      <c r="T21" s="25"/>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="T21" s="24"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="25"/>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="7"/>
       <c r="B22" s="23"/>
       <c r="C22" s="28"/>
@@ -1587,8 +1620,6 @@
       <c r="H22" s="26"/>
       <c r="I22" s="24"/>
       <c r="J22" s="25"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
       <c r="M22" s="23"/>
       <c r="N22" s="24"/>
       <c r="O22" s="23"/>
@@ -1596,9 +1627,11 @@
       <c r="Q22" s="23"/>
       <c r="R22" s="24"/>
       <c r="S22" s="23"/>
-      <c r="T22" s="25"/>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="T22" s="24"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="25"/>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="7"/>
       <c r="B23" s="23"/>
       <c r="C23" s="28"/>
@@ -1609,8 +1642,6 @@
       <c r="H23" s="26"/>
       <c r="I23" s="24"/>
       <c r="J23" s="25"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
       <c r="M23" s="23"/>
       <c r="N23" s="24"/>
       <c r="O23" s="23"/>
@@ -1618,9 +1649,11 @@
       <c r="Q23" s="23"/>
       <c r="R23" s="24"/>
       <c r="S23" s="23"/>
-      <c r="T23" s="25"/>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="T23" s="24"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="25"/>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="7"/>
       <c r="B24" s="23"/>
       <c r="C24" s="28"/>
@@ -1631,8 +1664,6 @@
       <c r="H24" s="26"/>
       <c r="I24" s="24"/>
       <c r="J24" s="25"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
       <c r="M24" s="23"/>
       <c r="N24" s="24"/>
       <c r="O24" s="23"/>
@@ -1640,9 +1671,11 @@
       <c r="Q24" s="23"/>
       <c r="R24" s="24"/>
       <c r="S24" s="23"/>
-      <c r="T24" s="25"/>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="T24" s="24"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="25"/>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="7"/>
       <c r="B25" s="23"/>
       <c r="C25" s="28"/>
@@ -1653,8 +1686,6 @@
       <c r="H25" s="26"/>
       <c r="I25" s="24"/>
       <c r="J25" s="25"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
       <c r="M25" s="23"/>
       <c r="N25" s="24"/>
       <c r="O25" s="23"/>
@@ -1662,9 +1693,11 @@
       <c r="Q25" s="23"/>
       <c r="R25" s="24"/>
       <c r="S25" s="23"/>
-      <c r="T25" s="25"/>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="T25" s="24"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="25"/>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="7"/>
       <c r="B26" s="23"/>
       <c r="C26" s="28"/>
@@ -1675,8 +1708,6 @@
       <c r="H26" s="26"/>
       <c r="I26" s="24"/>
       <c r="J26" s="25"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
       <c r="M26" s="23"/>
       <c r="N26" s="24"/>
       <c r="O26" s="23"/>
@@ -1684,9 +1715,11 @@
       <c r="Q26" s="23"/>
       <c r="R26" s="24"/>
       <c r="S26" s="23"/>
-      <c r="T26" s="25"/>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="T26" s="24"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="25"/>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="7"/>
       <c r="B27" s="23"/>
       <c r="C27" s="28"/>
@@ -1697,8 +1730,6 @@
       <c r="H27" s="26"/>
       <c r="I27" s="24"/>
       <c r="J27" s="25"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="24"/>
       <c r="M27" s="23"/>
       <c r="N27" s="24"/>
       <c r="O27" s="23"/>
@@ -1706,9 +1737,11 @@
       <c r="Q27" s="23"/>
       <c r="R27" s="24"/>
       <c r="S27" s="23"/>
-      <c r="T27" s="25"/>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="T27" s="24"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="25"/>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="7"/>
       <c r="B28" s="23"/>
       <c r="C28" s="28"/>
@@ -1719,8 +1752,6 @@
       <c r="H28" s="26"/>
       <c r="I28" s="24"/>
       <c r="J28" s="25"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="24"/>
       <c r="M28" s="23"/>
       <c r="N28" s="24"/>
       <c r="O28" s="23"/>
@@ -1728,9 +1759,11 @@
       <c r="Q28" s="23"/>
       <c r="R28" s="24"/>
       <c r="S28" s="23"/>
-      <c r="T28" s="25"/>
-    </row>
-    <row r="29" spans="1:20">
+      <c r="T28" s="24"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="25"/>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="7"/>
       <c r="B29" s="23"/>
       <c r="C29" s="28"/>
@@ -1741,8 +1774,6 @@
       <c r="H29" s="26"/>
       <c r="I29" s="24"/>
       <c r="J29" s="25"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="24"/>
       <c r="M29" s="23"/>
       <c r="N29" s="24"/>
       <c r="O29" s="23"/>
@@ -1750,9 +1781,11 @@
       <c r="Q29" s="23"/>
       <c r="R29" s="24"/>
       <c r="S29" s="23"/>
-      <c r="T29" s="25"/>
-    </row>
-    <row r="30" spans="1:20">
+      <c r="T29" s="24"/>
+      <c r="U29" s="23"/>
+      <c r="V29" s="25"/>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="7"/>
       <c r="B30" s="23"/>
       <c r="C30" s="28"/>
@@ -1763,8 +1796,6 @@
       <c r="H30" s="26"/>
       <c r="I30" s="24"/>
       <c r="J30" s="25"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="24"/>
       <c r="M30" s="23"/>
       <c r="N30" s="24"/>
       <c r="O30" s="23"/>
@@ -1772,9 +1803,11 @@
       <c r="Q30" s="23"/>
       <c r="R30" s="24"/>
       <c r="S30" s="23"/>
-      <c r="T30" s="25"/>
-    </row>
-    <row r="31" spans="1:20">
+      <c r="T30" s="24"/>
+      <c r="U30" s="23"/>
+      <c r="V30" s="25"/>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="7"/>
       <c r="B31" s="23"/>
       <c r="C31" s="28"/>
@@ -1785,8 +1818,6 @@
       <c r="H31" s="26"/>
       <c r="I31" s="24"/>
       <c r="J31" s="25"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="24"/>
       <c r="M31" s="23"/>
       <c r="N31" s="24"/>
       <c r="O31" s="23"/>
@@ -1794,9 +1825,11 @@
       <c r="Q31" s="23"/>
       <c r="R31" s="24"/>
       <c r="S31" s="23"/>
-      <c r="T31" s="25"/>
-    </row>
-    <row r="32" spans="1:20">
+      <c r="T31" s="24"/>
+      <c r="U31" s="23"/>
+      <c r="V31" s="25"/>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="7"/>
       <c r="B32" s="23"/>
       <c r="C32" s="28"/>
@@ -1807,8 +1840,6 @@
       <c r="H32" s="26"/>
       <c r="I32" s="24"/>
       <c r="J32" s="25"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="24"/>
       <c r="M32" s="23"/>
       <c r="N32" s="24"/>
       <c r="O32" s="23"/>
@@ -1816,9 +1847,11 @@
       <c r="Q32" s="23"/>
       <c r="R32" s="24"/>
       <c r="S32" s="23"/>
-      <c r="T32" s="25"/>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="T32" s="24"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="25"/>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="7"/>
       <c r="B33" s="23"/>
       <c r="C33" s="28"/>
@@ -1829,8 +1862,6 @@
       <c r="H33" s="26"/>
       <c r="I33" s="24"/>
       <c r="J33" s="25"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="24"/>
       <c r="M33" s="23"/>
       <c r="N33" s="24"/>
       <c r="O33" s="23"/>
@@ -1838,9 +1869,11 @@
       <c r="Q33" s="23"/>
       <c r="R33" s="24"/>
       <c r="S33" s="23"/>
-      <c r="T33" s="25"/>
-    </row>
-    <row r="34" spans="1:20">
+      <c r="T33" s="24"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="25"/>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" s="7"/>
       <c r="B34" s="23"/>
       <c r="C34" s="28"/>
@@ -1851,8 +1884,6 @@
       <c r="H34" s="26"/>
       <c r="I34" s="24"/>
       <c r="J34" s="25"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="24"/>
       <c r="M34" s="23"/>
       <c r="N34" s="24"/>
       <c r="O34" s="23"/>
@@ -1860,9 +1891,11 @@
       <c r="Q34" s="23"/>
       <c r="R34" s="24"/>
       <c r="S34" s="23"/>
-      <c r="T34" s="25"/>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="T34" s="24"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="25"/>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" s="7"/>
       <c r="B35" s="23"/>
       <c r="C35" s="28"/>
@@ -1873,8 +1906,6 @@
       <c r="H35" s="26"/>
       <c r="I35" s="24"/>
       <c r="J35" s="25"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="24"/>
       <c r="M35" s="23"/>
       <c r="N35" s="24"/>
       <c r="O35" s="23"/>
@@ -1882,9 +1913,11 @@
       <c r="Q35" s="23"/>
       <c r="R35" s="24"/>
       <c r="S35" s="23"/>
-      <c r="T35" s="25"/>
-    </row>
-    <row r="36" spans="1:20">
+      <c r="T35" s="24"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="25"/>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" s="7"/>
       <c r="B36" s="23"/>
       <c r="C36" s="28"/>
@@ -1895,8 +1928,6 @@
       <c r="H36" s="26"/>
       <c r="I36" s="24"/>
       <c r="J36" s="25"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="24"/>
       <c r="M36" s="23"/>
       <c r="N36" s="24"/>
       <c r="O36" s="23"/>
@@ -1904,9 +1935,11 @@
       <c r="Q36" s="23"/>
       <c r="R36" s="24"/>
       <c r="S36" s="23"/>
-      <c r="T36" s="25"/>
-    </row>
-    <row r="37" spans="1:20">
+      <c r="T36" s="24"/>
+      <c r="U36" s="23"/>
+      <c r="V36" s="25"/>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" s="7"/>
       <c r="B37" s="23"/>
       <c r="C37" s="28"/>
@@ -1917,8 +1950,6 @@
       <c r="H37" s="26"/>
       <c r="I37" s="24"/>
       <c r="J37" s="25"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="24"/>
       <c r="M37" s="23"/>
       <c r="N37" s="24"/>
       <c r="O37" s="23"/>
@@ -1926,9 +1957,11 @@
       <c r="Q37" s="23"/>
       <c r="R37" s="24"/>
       <c r="S37" s="23"/>
-      <c r="T37" s="25"/>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="T37" s="24"/>
+      <c r="U37" s="23"/>
+      <c r="V37" s="25"/>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" s="7"/>
       <c r="B38" s="23"/>
       <c r="C38" s="28"/>
@@ -1939,8 +1972,6 @@
       <c r="H38" s="26"/>
       <c r="I38" s="24"/>
       <c r="J38" s="25"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="24"/>
       <c r="M38" s="23"/>
       <c r="N38" s="24"/>
       <c r="O38" s="23"/>
@@ -1948,9 +1979,11 @@
       <c r="Q38" s="23"/>
       <c r="R38" s="24"/>
       <c r="S38" s="23"/>
-      <c r="T38" s="25"/>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="T38" s="24"/>
+      <c r="U38" s="23"/>
+      <c r="V38" s="25"/>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" s="7"/>
       <c r="B39" s="23"/>
       <c r="C39" s="28"/>
@@ -1961,8 +1994,8 @@
       <c r="H39" s="26"/>
       <c r="I39" s="28"/>
       <c r="J39" s="25"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="24"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
       <c r="M39" s="23"/>
       <c r="N39" s="24"/>
       <c r="O39" s="23"/>
@@ -1970,9 +2003,11 @@
       <c r="Q39" s="23"/>
       <c r="R39" s="24"/>
       <c r="S39" s="23"/>
-      <c r="T39" s="25"/>
-    </row>
-    <row r="40" spans="1:20">
+      <c r="T39" s="24"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="25"/>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" s="7"/>
       <c r="B40" s="23"/>
       <c r="C40" s="28"/>
@@ -1983,8 +2018,6 @@
       <c r="H40" s="26"/>
       <c r="I40" s="28"/>
       <c r="J40" s="25"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="24"/>
       <c r="M40" s="23"/>
       <c r="N40" s="24"/>
       <c r="O40" s="23"/>
@@ -1992,9 +2025,11 @@
       <c r="Q40" s="23"/>
       <c r="R40" s="24"/>
       <c r="S40" s="23"/>
-      <c r="T40" s="25"/>
-    </row>
-    <row r="41" spans="1:20">
+      <c r="T40" s="24"/>
+      <c r="U40" s="23"/>
+      <c r="V40" s="25"/>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" s="7"/>
       <c r="B41" s="23"/>
       <c r="C41" s="24"/>
@@ -2005,8 +2040,8 @@
       <c r="H41" s="26"/>
       <c r="I41" s="28"/>
       <c r="J41" s="25"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="24"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
       <c r="M41" s="23"/>
       <c r="N41" s="24"/>
       <c r="O41" s="23"/>
@@ -2014,9 +2049,11 @@
       <c r="Q41" s="23"/>
       <c r="R41" s="24"/>
       <c r="S41" s="23"/>
-      <c r="T41" s="25"/>
-    </row>
-    <row r="42" spans="1:20">
+      <c r="T41" s="24"/>
+      <c r="U41" s="23"/>
+      <c r="V41" s="25"/>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" s="7"/>
       <c r="B42" s="23"/>
       <c r="C42" s="24"/>
@@ -2027,8 +2064,8 @@
       <c r="H42" s="26"/>
       <c r="I42" s="28"/>
       <c r="J42" s="25"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="24"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
       <c r="M42" s="23"/>
       <c r="N42" s="24"/>
       <c r="O42" s="23"/>
@@ -2036,9 +2073,11 @@
       <c r="Q42" s="23"/>
       <c r="R42" s="24"/>
       <c r="S42" s="23"/>
-      <c r="T42" s="25"/>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="T42" s="24"/>
+      <c r="U42" s="23"/>
+      <c r="V42" s="25"/>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43" s="7"/>
       <c r="B43" s="23"/>
       <c r="C43" s="24"/>
@@ -2049,8 +2088,6 @@
       <c r="H43" s="26"/>
       <c r="I43" s="24"/>
       <c r="J43" s="25"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="24"/>
       <c r="M43" s="23"/>
       <c r="N43" s="24"/>
       <c r="O43" s="23"/>
@@ -2058,9 +2095,11 @@
       <c r="Q43" s="23"/>
       <c r="R43" s="24"/>
       <c r="S43" s="23"/>
-      <c r="T43" s="25"/>
-    </row>
-    <row r="44" spans="1:20">
+      <c r="T43" s="24"/>
+      <c r="U43" s="23"/>
+      <c r="V43" s="25"/>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" s="7"/>
       <c r="B44" s="23"/>
       <c r="C44" s="28"/>
@@ -2071,8 +2110,6 @@
       <c r="H44" s="26"/>
       <c r="I44" s="24"/>
       <c r="J44" s="25"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="24"/>
       <c r="M44" s="23"/>
       <c r="N44" s="24"/>
       <c r="O44" s="23"/>
@@ -2080,9 +2117,11 @@
       <c r="Q44" s="23"/>
       <c r="R44" s="24"/>
       <c r="S44" s="23"/>
-      <c r="T44" s="25"/>
-    </row>
-    <row r="45" spans="1:20">
+      <c r="T44" s="24"/>
+      <c r="U44" s="23"/>
+      <c r="V44" s="25"/>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" s="7"/>
       <c r="B45" s="23"/>
       <c r="C45" s="28"/>
@@ -2093,8 +2132,6 @@
       <c r="H45" s="26"/>
       <c r="I45" s="24"/>
       <c r="J45" s="25"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="24"/>
       <c r="M45" s="23"/>
       <c r="N45" s="24"/>
       <c r="O45" s="23"/>
@@ -2102,9 +2139,11 @@
       <c r="Q45" s="23"/>
       <c r="R45" s="24"/>
       <c r="S45" s="23"/>
-      <c r="T45" s="25"/>
-    </row>
-    <row r="46" spans="1:20">
+      <c r="T45" s="24"/>
+      <c r="U45" s="23"/>
+      <c r="V45" s="25"/>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" s="7"/>
       <c r="B46" s="23"/>
       <c r="C46" s="24"/>
@@ -2115,8 +2154,6 @@
       <c r="H46" s="26"/>
       <c r="I46" s="24"/>
       <c r="J46" s="25"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="24"/>
       <c r="M46" s="23"/>
       <c r="N46" s="24"/>
       <c r="O46" s="23"/>
@@ -2124,9 +2161,11 @@
       <c r="Q46" s="23"/>
       <c r="R46" s="24"/>
       <c r="S46" s="23"/>
-      <c r="T46" s="25"/>
-    </row>
-    <row r="47" spans="1:20">
+      <c r="T46" s="24"/>
+      <c r="U46" s="23"/>
+      <c r="V46" s="25"/>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" s="7"/>
       <c r="B47" s="23"/>
       <c r="C47" s="24"/>
@@ -2137,8 +2176,6 @@
       <c r="H47" s="26"/>
       <c r="I47" s="24"/>
       <c r="J47" s="25"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="24"/>
       <c r="M47" s="23"/>
       <c r="N47" s="24"/>
       <c r="O47" s="23"/>
@@ -2146,9 +2183,11 @@
       <c r="Q47" s="23"/>
       <c r="R47" s="24"/>
       <c r="S47" s="23"/>
-      <c r="T47" s="25"/>
-    </row>
-    <row r="48" spans="1:20">
+      <c r="T47" s="24"/>
+      <c r="U47" s="23"/>
+      <c r="V47" s="25"/>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" s="7"/>
       <c r="B48" s="23"/>
       <c r="C48" s="24"/>
@@ -2159,8 +2198,6 @@
       <c r="H48" s="26"/>
       <c r="I48" s="24"/>
       <c r="J48" s="25"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="24"/>
       <c r="M48" s="23"/>
       <c r="N48" s="24"/>
       <c r="O48" s="23"/>
@@ -2168,9 +2205,11 @@
       <c r="Q48" s="23"/>
       <c r="R48" s="24"/>
       <c r="S48" s="23"/>
-      <c r="T48" s="25"/>
-    </row>
-    <row r="49" spans="1:20">
+      <c r="T48" s="24"/>
+      <c r="U48" s="23"/>
+      <c r="V48" s="25"/>
+    </row>
+    <row r="49" spans="1:22">
       <c r="A49" s="7"/>
       <c r="B49" s="23"/>
       <c r="C49" s="24"/>
@@ -2181,8 +2220,6 @@
       <c r="H49" s="26"/>
       <c r="I49" s="24"/>
       <c r="J49" s="25"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="24"/>
       <c r="M49" s="23"/>
       <c r="N49" s="24"/>
       <c r="O49" s="23"/>
@@ -2190,9 +2227,11 @@
       <c r="Q49" s="23"/>
       <c r="R49" s="24"/>
       <c r="S49" s="23"/>
-      <c r="T49" s="25"/>
-    </row>
-    <row r="50" spans="1:20">
+      <c r="T49" s="24"/>
+      <c r="U49" s="23"/>
+      <c r="V49" s="25"/>
+    </row>
+    <row r="50" spans="1:22">
       <c r="A50" s="7"/>
       <c r="B50" s="23"/>
       <c r="C50" s="28"/>
@@ -2203,8 +2242,6 @@
       <c r="H50" s="26"/>
       <c r="I50" s="24"/>
       <c r="J50" s="25"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="24"/>
       <c r="M50" s="23"/>
       <c r="N50" s="24"/>
       <c r="O50" s="23"/>
@@ -2212,9 +2249,11 @@
       <c r="Q50" s="23"/>
       <c r="R50" s="24"/>
       <c r="S50" s="23"/>
-      <c r="T50" s="25"/>
-    </row>
-    <row r="51" spans="1:20">
+      <c r="T50" s="24"/>
+      <c r="U50" s="23"/>
+      <c r="V50" s="25"/>
+    </row>
+    <row r="51" spans="1:22">
       <c r="A51" s="7"/>
       <c r="B51" s="23"/>
       <c r="C51" s="28"/>
@@ -2225,8 +2264,6 @@
       <c r="H51" s="26"/>
       <c r="I51" s="24"/>
       <c r="J51" s="25"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="24"/>
       <c r="M51" s="23"/>
       <c r="N51" s="24"/>
       <c r="O51" s="23"/>
@@ -2234,9 +2271,11 @@
       <c r="Q51" s="23"/>
       <c r="R51" s="24"/>
       <c r="S51" s="23"/>
-      <c r="T51" s="25"/>
-    </row>
-    <row r="52" spans="1:20">
+      <c r="T51" s="24"/>
+      <c r="U51" s="23"/>
+      <c r="V51" s="25"/>
+    </row>
+    <row r="52" spans="1:22">
       <c r="A52" s="7"/>
       <c r="B52" s="23"/>
       <c r="C52" s="24"/>
@@ -2247,8 +2286,6 @@
       <c r="H52" s="26"/>
       <c r="I52" s="24"/>
       <c r="J52" s="25"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="24"/>
       <c r="M52" s="23"/>
       <c r="N52" s="24"/>
       <c r="O52" s="23"/>
@@ -2256,9 +2293,11 @@
       <c r="Q52" s="23"/>
       <c r="R52" s="24"/>
       <c r="S52" s="23"/>
-      <c r="T52" s="25"/>
-    </row>
-    <row r="53" spans="1:20">
+      <c r="T52" s="24"/>
+      <c r="U52" s="23"/>
+      <c r="V52" s="25"/>
+    </row>
+    <row r="53" spans="1:22">
       <c r="A53" s="7"/>
       <c r="B53" s="23"/>
       <c r="C53" s="24"/>
@@ -2269,8 +2308,6 @@
       <c r="H53" s="26"/>
       <c r="I53" s="24"/>
       <c r="J53" s="25"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="24"/>
       <c r="M53" s="23"/>
       <c r="N53" s="24"/>
       <c r="O53" s="23"/>
@@ -2278,9 +2315,11 @@
       <c r="Q53" s="23"/>
       <c r="R53" s="24"/>
       <c r="S53" s="23"/>
-      <c r="T53" s="25"/>
-    </row>
-    <row r="54" spans="1:20">
+      <c r="T53" s="24"/>
+      <c r="U53" s="23"/>
+      <c r="V53" s="25"/>
+    </row>
+    <row r="54" spans="1:22">
       <c r="A54" s="7"/>
       <c r="B54" s="23"/>
       <c r="C54" s="24"/>
@@ -2291,8 +2330,6 @@
       <c r="H54" s="26"/>
       <c r="I54" s="24"/>
       <c r="J54" s="25"/>
-      <c r="K54" s="23"/>
-      <c r="L54" s="24"/>
       <c r="M54" s="23"/>
       <c r="N54" s="24"/>
       <c r="O54" s="23"/>
@@ -2300,9 +2337,11 @@
       <c r="Q54" s="23"/>
       <c r="R54" s="24"/>
       <c r="S54" s="23"/>
-      <c r="T54" s="25"/>
-    </row>
-    <row r="55" spans="1:20">
+      <c r="T54" s="24"/>
+      <c r="U54" s="23"/>
+      <c r="V54" s="25"/>
+    </row>
+    <row r="55" spans="1:22">
       <c r="A55" s="7"/>
       <c r="B55" s="23"/>
       <c r="C55" s="28"/>
@@ -2313,8 +2352,6 @@
       <c r="H55" s="26"/>
       <c r="I55" s="24"/>
       <c r="J55" s="25"/>
-      <c r="K55" s="23"/>
-      <c r="L55" s="24"/>
       <c r="M55" s="23"/>
       <c r="N55" s="24"/>
       <c r="O55" s="23"/>
@@ -2322,9 +2359,11 @@
       <c r="Q55" s="23"/>
       <c r="R55" s="24"/>
       <c r="S55" s="23"/>
-      <c r="T55" s="25"/>
-    </row>
-    <row r="56" spans="1:20">
+      <c r="T55" s="24"/>
+      <c r="U55" s="23"/>
+      <c r="V55" s="25"/>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" s="7"/>
       <c r="B56" s="23"/>
       <c r="C56" s="28"/>
@@ -2335,8 +2374,6 @@
       <c r="H56" s="26"/>
       <c r="I56" s="24"/>
       <c r="J56" s="25"/>
-      <c r="K56" s="23"/>
-      <c r="L56" s="24"/>
       <c r="M56" s="23"/>
       <c r="N56" s="24"/>
       <c r="O56" s="23"/>
@@ -2344,9 +2381,11 @@
       <c r="Q56" s="23"/>
       <c r="R56" s="24"/>
       <c r="S56" s="23"/>
-      <c r="T56" s="25"/>
-    </row>
-    <row r="57" spans="1:20">
+      <c r="T56" s="24"/>
+      <c r="U56" s="23"/>
+      <c r="V56" s="25"/>
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" s="7"/>
       <c r="B57" s="23"/>
       <c r="C57" s="24"/>
@@ -2357,8 +2396,6 @@
       <c r="H57" s="26"/>
       <c r="I57" s="24"/>
       <c r="J57" s="25"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="24"/>
       <c r="M57" s="23"/>
       <c r="N57" s="24"/>
       <c r="O57" s="23"/>
@@ -2366,9 +2403,11 @@
       <c r="Q57" s="23"/>
       <c r="R57" s="24"/>
       <c r="S57" s="23"/>
-      <c r="T57" s="25"/>
-    </row>
-    <row r="58" spans="1:20">
+      <c r="T57" s="24"/>
+      <c r="U57" s="23"/>
+      <c r="V57" s="25"/>
+    </row>
+    <row r="58" spans="1:22">
       <c r="A58" s="7"/>
       <c r="B58" s="23"/>
       <c r="C58" s="28"/>
@@ -2379,8 +2418,6 @@
       <c r="H58" s="26"/>
       <c r="I58" s="24"/>
       <c r="J58" s="25"/>
-      <c r="K58" s="23"/>
-      <c r="L58" s="24"/>
       <c r="M58" s="23"/>
       <c r="N58" s="24"/>
       <c r="O58" s="23"/>
@@ -2388,9 +2425,11 @@
       <c r="Q58" s="23"/>
       <c r="R58" s="24"/>
       <c r="S58" s="23"/>
-      <c r="T58" s="25"/>
-    </row>
-    <row r="59" spans="1:20">
+      <c r="T58" s="24"/>
+      <c r="U58" s="23"/>
+      <c r="V58" s="25"/>
+    </row>
+    <row r="59" spans="1:22">
       <c r="A59" s="7"/>
       <c r="B59" s="23"/>
       <c r="C59" s="28"/>
@@ -2401,8 +2440,6 @@
       <c r="H59" s="26"/>
       <c r="I59" s="24"/>
       <c r="J59" s="25"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="24"/>
       <c r="M59" s="23"/>
       <c r="N59" s="24"/>
       <c r="O59" s="23"/>
@@ -2410,9 +2447,11 @@
       <c r="Q59" s="23"/>
       <c r="R59" s="24"/>
       <c r="S59" s="23"/>
-      <c r="T59" s="25"/>
-    </row>
-    <row r="60" spans="1:20">
+      <c r="T59" s="24"/>
+      <c r="U59" s="23"/>
+      <c r="V59" s="25"/>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" s="7"/>
       <c r="B60" s="23"/>
       <c r="C60" s="28"/>
@@ -2423,8 +2462,6 @@
       <c r="H60" s="26"/>
       <c r="I60" s="24"/>
       <c r="J60" s="25"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="24"/>
       <c r="M60" s="23"/>
       <c r="N60" s="24"/>
       <c r="O60" s="23"/>
@@ -2432,9 +2469,11 @@
       <c r="Q60" s="23"/>
       <c r="R60" s="24"/>
       <c r="S60" s="23"/>
-      <c r="T60" s="25"/>
-    </row>
-    <row r="61" spans="1:20">
+      <c r="T60" s="24"/>
+      <c r="U60" s="23"/>
+      <c r="V60" s="25"/>
+    </row>
+    <row r="61" spans="1:22">
       <c r="A61" s="7"/>
       <c r="B61" s="23"/>
       <c r="C61" s="28"/>
@@ -2445,8 +2484,6 @@
       <c r="H61" s="26"/>
       <c r="I61" s="24"/>
       <c r="J61" s="25"/>
-      <c r="K61" s="23"/>
-      <c r="L61" s="24"/>
       <c r="M61" s="23"/>
       <c r="N61" s="24"/>
       <c r="O61" s="23"/>
@@ -2454,9 +2491,11 @@
       <c r="Q61" s="23"/>
       <c r="R61" s="24"/>
       <c r="S61" s="23"/>
-      <c r="T61" s="25"/>
-    </row>
-    <row r="62" spans="1:20">
+      <c r="T61" s="24"/>
+      <c r="U61" s="23"/>
+      <c r="V61" s="25"/>
+    </row>
+    <row r="62" spans="1:22">
       <c r="A62" s="7"/>
       <c r="B62" s="23"/>
       <c r="C62" s="28"/>
@@ -2467,8 +2506,6 @@
       <c r="H62" s="26"/>
       <c r="I62" s="24"/>
       <c r="J62" s="25"/>
-      <c r="K62" s="23"/>
-      <c r="L62" s="24"/>
       <c r="M62" s="23"/>
       <c r="N62" s="24"/>
       <c r="O62" s="23"/>
@@ -2476,9 +2513,11 @@
       <c r="Q62" s="23"/>
       <c r="R62" s="24"/>
       <c r="S62" s="23"/>
-      <c r="T62" s="25"/>
-    </row>
-    <row r="63" spans="1:20" s="24" customFormat="1">
+      <c r="T62" s="24"/>
+      <c r="U62" s="23"/>
+      <c r="V62" s="25"/>
+    </row>
+    <row r="63" spans="1:22" s="24" customFormat="1">
       <c r="B63" s="23"/>
       <c r="C63" s="28"/>
       <c r="D63" s="28"/>
@@ -2486,14 +2525,14 @@
       <c r="G63" s="25"/>
       <c r="H63" s="26"/>
       <c r="J63" s="25"/>
-      <c r="K63" s="23"/>
       <c r="M63" s="23"/>
       <c r="O63" s="23"/>
       <c r="Q63" s="23"/>
       <c r="S63" s="23"/>
-      <c r="T63" s="25"/>
-    </row>
-    <row r="64" spans="1:20">
+      <c r="U63" s="23"/>
+      <c r="V63" s="25"/>
+    </row>
+    <row r="64" spans="1:22">
       <c r="A64" s="7"/>
       <c r="B64" s="23"/>
       <c r="C64" s="28"/>
@@ -2504,8 +2543,6 @@
       <c r="H64" s="26"/>
       <c r="I64" s="24"/>
       <c r="J64" s="25"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="24"/>
       <c r="M64" s="23"/>
       <c r="N64" s="24"/>
       <c r="O64" s="23"/>
@@ -2513,9 +2550,11 @@
       <c r="Q64" s="23"/>
       <c r="R64" s="24"/>
       <c r="S64" s="23"/>
-      <c r="T64" s="25"/>
-    </row>
-    <row r="65" spans="1:20" s="24" customFormat="1">
+      <c r="T64" s="24"/>
+      <c r="U64" s="23"/>
+      <c r="V64" s="25"/>
+    </row>
+    <row r="65" spans="1:22" s="24" customFormat="1">
       <c r="B65" s="23"/>
       <c r="C65" s="28"/>
       <c r="D65" s="28"/>
@@ -2523,14 +2562,14 @@
       <c r="G65" s="25"/>
       <c r="H65" s="26"/>
       <c r="J65" s="25"/>
-      <c r="K65" s="23"/>
       <c r="M65" s="23"/>
       <c r="O65" s="23"/>
       <c r="Q65" s="23"/>
       <c r="S65" s="23"/>
-      <c r="T65" s="25"/>
-    </row>
-    <row r="66" spans="1:20" s="24" customFormat="1">
+      <c r="U65" s="23"/>
+      <c r="V65" s="25"/>
+    </row>
+    <row r="66" spans="1:22" s="24" customFormat="1">
       <c r="B66" s="23"/>
       <c r="C66" s="28"/>
       <c r="D66" s="28"/>
@@ -2538,14 +2577,14 @@
       <c r="G66" s="25"/>
       <c r="H66" s="26"/>
       <c r="J66" s="25"/>
-      <c r="K66" s="23"/>
       <c r="M66" s="23"/>
       <c r="O66" s="23"/>
       <c r="Q66" s="23"/>
       <c r="S66" s="23"/>
-      <c r="T66" s="25"/>
-    </row>
-    <row r="67" spans="1:20">
+      <c r="U66" s="23"/>
+      <c r="V66" s="25"/>
+    </row>
+    <row r="67" spans="1:22">
       <c r="A67" s="7"/>
       <c r="B67" s="23"/>
       <c r="C67" s="28"/>
@@ -2556,8 +2595,6 @@
       <c r="H67" s="26"/>
       <c r="I67" s="24"/>
       <c r="J67" s="25"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="24"/>
       <c r="M67" s="23"/>
       <c r="N67" s="24"/>
       <c r="O67" s="23"/>
@@ -2565,9 +2602,11 @@
       <c r="Q67" s="23"/>
       <c r="R67" s="24"/>
       <c r="S67" s="23"/>
-      <c r="T67" s="25"/>
-    </row>
-    <row r="68" spans="1:20">
+      <c r="T67" s="24"/>
+      <c r="U67" s="23"/>
+      <c r="V67" s="25"/>
+    </row>
+    <row r="68" spans="1:22">
       <c r="A68" s="7"/>
       <c r="B68" s="23"/>
       <c r="C68" s="28"/>
@@ -2578,8 +2617,6 @@
       <c r="H68" s="26"/>
       <c r="I68" s="24"/>
       <c r="J68" s="25"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="24"/>
       <c r="M68" s="23"/>
       <c r="N68" s="24"/>
       <c r="O68" s="23"/>
@@ -2587,9 +2624,11 @@
       <c r="Q68" s="23"/>
       <c r="R68" s="24"/>
       <c r="S68" s="23"/>
-      <c r="T68" s="25"/>
-    </row>
-    <row r="69" spans="1:20">
+      <c r="T68" s="24"/>
+      <c r="U68" s="23"/>
+      <c r="V68" s="25"/>
+    </row>
+    <row r="69" spans="1:22">
       <c r="A69" s="7"/>
       <c r="B69" s="23"/>
       <c r="C69" s="28"/>
@@ -2600,8 +2639,6 @@
       <c r="H69" s="26"/>
       <c r="I69" s="28"/>
       <c r="J69" s="25"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="24"/>
       <c r="M69" s="23"/>
       <c r="N69" s="24"/>
       <c r="O69" s="23"/>
@@ -2609,9 +2646,11 @@
       <c r="Q69" s="23"/>
       <c r="R69" s="24"/>
       <c r="S69" s="23"/>
-      <c r="T69" s="25"/>
-    </row>
-    <row r="70" spans="1:20">
+      <c r="T69" s="24"/>
+      <c r="U69" s="23"/>
+      <c r="V69" s="25"/>
+    </row>
+    <row r="70" spans="1:22">
       <c r="A70" s="7"/>
       <c r="B70" s="23"/>
       <c r="C70" s="28"/>
@@ -2622,8 +2661,6 @@
       <c r="H70" s="26"/>
       <c r="I70" s="28"/>
       <c r="J70" s="25"/>
-      <c r="K70" s="23"/>
-      <c r="L70" s="24"/>
       <c r="M70" s="23"/>
       <c r="N70" s="24"/>
       <c r="O70" s="23"/>
@@ -2631,9 +2668,11 @@
       <c r="Q70" s="23"/>
       <c r="R70" s="24"/>
       <c r="S70" s="23"/>
-      <c r="T70" s="25"/>
-    </row>
-    <row r="71" spans="1:20">
+      <c r="T70" s="24"/>
+      <c r="U70" s="23"/>
+      <c r="V70" s="25"/>
+    </row>
+    <row r="71" spans="1:22">
       <c r="A71" s="7"/>
       <c r="B71" s="23"/>
       <c r="C71" s="28"/>
@@ -2644,8 +2683,6 @@
       <c r="H71" s="26"/>
       <c r="I71" s="24"/>
       <c r="J71" s="25"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="24"/>
       <c r="M71" s="23"/>
       <c r="N71" s="24"/>
       <c r="O71" s="23"/>
@@ -2653,9 +2690,11 @@
       <c r="Q71" s="23"/>
       <c r="R71" s="24"/>
       <c r="S71" s="23"/>
-      <c r="T71" s="25"/>
-    </row>
-    <row r="72" spans="1:20">
+      <c r="T71" s="24"/>
+      <c r="U71" s="23"/>
+      <c r="V71" s="25"/>
+    </row>
+    <row r="72" spans="1:22">
       <c r="A72" s="7"/>
       <c r="B72" s="23"/>
       <c r="C72" s="28"/>
@@ -2666,8 +2705,6 @@
       <c r="H72" s="26"/>
       <c r="I72" s="24"/>
       <c r="J72" s="25"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="24"/>
       <c r="M72" s="23"/>
       <c r="N72" s="24"/>
       <c r="O72" s="23"/>
@@ -2675,9 +2712,11 @@
       <c r="Q72" s="23"/>
       <c r="R72" s="24"/>
       <c r="S72" s="23"/>
-      <c r="T72" s="25"/>
-    </row>
-    <row r="73" spans="1:20">
+      <c r="T72" s="24"/>
+      <c r="U72" s="23"/>
+      <c r="V72" s="25"/>
+    </row>
+    <row r="73" spans="1:22">
       <c r="A73" s="7"/>
       <c r="B73" s="23"/>
       <c r="C73" s="28"/>
@@ -2688,8 +2727,6 @@
       <c r="H73" s="26"/>
       <c r="I73" s="24"/>
       <c r="J73" s="25"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="24"/>
       <c r="M73" s="23"/>
       <c r="N73" s="24"/>
       <c r="O73" s="23"/>
@@ -2697,9 +2734,11 @@
       <c r="Q73" s="23"/>
       <c r="R73" s="24"/>
       <c r="S73" s="23"/>
-      <c r="T73" s="25"/>
-    </row>
-    <row r="74" spans="1:20">
+      <c r="T73" s="24"/>
+      <c r="U73" s="23"/>
+      <c r="V73" s="25"/>
+    </row>
+    <row r="74" spans="1:22">
       <c r="A74" s="7"/>
       <c r="B74" s="23"/>
       <c r="C74" s="28"/>
@@ -2710,8 +2749,6 @@
       <c r="H74" s="26"/>
       <c r="I74" s="24"/>
       <c r="J74" s="25"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="24"/>
       <c r="M74" s="23"/>
       <c r="N74" s="24"/>
       <c r="O74" s="23"/>
@@ -2719,9 +2756,11 @@
       <c r="Q74" s="23"/>
       <c r="R74" s="24"/>
       <c r="S74" s="23"/>
-      <c r="T74" s="25"/>
-    </row>
-    <row r="75" spans="1:20">
+      <c r="T74" s="24"/>
+      <c r="U74" s="23"/>
+      <c r="V74" s="25"/>
+    </row>
+    <row r="75" spans="1:22">
       <c r="A75" s="7"/>
       <c r="B75" s="23"/>
       <c r="C75" s="24"/>
@@ -2732,8 +2771,6 @@
       <c r="H75" s="26"/>
       <c r="I75" s="24"/>
       <c r="J75" s="25"/>
-      <c r="K75" s="23"/>
-      <c r="L75" s="24"/>
       <c r="M75" s="23"/>
       <c r="N75" s="24"/>
       <c r="O75" s="23"/>
@@ -2741,9 +2778,11 @@
       <c r="Q75" s="23"/>
       <c r="R75" s="24"/>
       <c r="S75" s="23"/>
-      <c r="T75" s="25"/>
-    </row>
-    <row r="76" spans="1:20">
+      <c r="T75" s="24"/>
+      <c r="U75" s="23"/>
+      <c r="V75" s="25"/>
+    </row>
+    <row r="76" spans="1:22">
       <c r="A76" s="7"/>
       <c r="B76" s="23"/>
       <c r="C76" s="24"/>
@@ -2754,8 +2793,6 @@
       <c r="H76" s="26"/>
       <c r="I76" s="24"/>
       <c r="J76" s="25"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="24"/>
       <c r="M76" s="23"/>
       <c r="N76" s="24"/>
       <c r="O76" s="23"/>
@@ -2763,9 +2800,11 @@
       <c r="Q76" s="23"/>
       <c r="R76" s="24"/>
       <c r="S76" s="23"/>
-      <c r="T76" s="25"/>
-    </row>
-    <row r="77" spans="1:20">
+      <c r="T76" s="24"/>
+      <c r="U76" s="23"/>
+      <c r="V76" s="25"/>
+    </row>
+    <row r="77" spans="1:22">
       <c r="A77" s="7"/>
       <c r="B77" s="23"/>
       <c r="C77" s="28"/>
@@ -2776,8 +2815,6 @@
       <c r="H77" s="26"/>
       <c r="I77" s="24"/>
       <c r="J77" s="25"/>
-      <c r="K77" s="23"/>
-      <c r="L77" s="24"/>
       <c r="M77" s="23"/>
       <c r="N77" s="24"/>
       <c r="O77" s="23"/>
@@ -2785,9 +2822,11 @@
       <c r="Q77" s="23"/>
       <c r="R77" s="24"/>
       <c r="S77" s="23"/>
-      <c r="T77" s="25"/>
-    </row>
-    <row r="78" spans="1:20">
+      <c r="T77" s="24"/>
+      <c r="U77" s="23"/>
+      <c r="V77" s="25"/>
+    </row>
+    <row r="78" spans="1:22">
       <c r="A78" s="7"/>
       <c r="B78" s="23"/>
       <c r="C78" s="28"/>
@@ -2798,8 +2837,6 @@
       <c r="H78" s="26"/>
       <c r="I78" s="24"/>
       <c r="J78" s="25"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="24"/>
       <c r="M78" s="23"/>
       <c r="N78" s="24"/>
       <c r="O78" s="23"/>
@@ -2807,9 +2844,11 @@
       <c r="Q78" s="23"/>
       <c r="R78" s="24"/>
       <c r="S78" s="23"/>
-      <c r="T78" s="25"/>
-    </row>
-    <row r="79" spans="1:20">
+      <c r="T78" s="24"/>
+      <c r="U78" s="23"/>
+      <c r="V78" s="25"/>
+    </row>
+    <row r="79" spans="1:22">
       <c r="A79" s="7"/>
       <c r="B79" s="23"/>
       <c r="C79" s="28"/>
@@ -2820,8 +2859,6 @@
       <c r="H79" s="26"/>
       <c r="I79" s="28"/>
       <c r="J79" s="25"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="24"/>
       <c r="M79" s="23"/>
       <c r="N79" s="24"/>
       <c r="O79" s="23"/>
@@ -2829,9 +2866,11 @@
       <c r="Q79" s="23"/>
       <c r="R79" s="24"/>
       <c r="S79" s="23"/>
-      <c r="T79" s="25"/>
-    </row>
-    <row r="80" spans="1:20">
+      <c r="T79" s="24"/>
+      <c r="U79" s="23"/>
+      <c r="V79" s="25"/>
+    </row>
+    <row r="80" spans="1:22">
       <c r="A80" s="7"/>
       <c r="B80" s="23"/>
       <c r="C80" s="28"/>
@@ -2842,8 +2881,6 @@
       <c r="H80" s="26"/>
       <c r="I80" s="28"/>
       <c r="J80" s="25"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="24"/>
       <c r="M80" s="23"/>
       <c r="N80" s="24"/>
       <c r="O80" s="23"/>
@@ -2851,9 +2888,11 @@
       <c r="Q80" s="23"/>
       <c r="R80" s="24"/>
       <c r="S80" s="23"/>
-      <c r="T80" s="25"/>
-    </row>
-    <row r="81" spans="1:20">
+      <c r="T80" s="24"/>
+      <c r="U80" s="23"/>
+      <c r="V80" s="25"/>
+    </row>
+    <row r="81" spans="1:22">
       <c r="A81" s="7"/>
       <c r="B81" s="23"/>
       <c r="C81" s="28"/>
@@ -2864,8 +2903,6 @@
       <c r="H81" s="26"/>
       <c r="I81" s="24"/>
       <c r="J81" s="25"/>
-      <c r="K81" s="23"/>
-      <c r="L81" s="24"/>
       <c r="M81" s="23"/>
       <c r="N81" s="24"/>
       <c r="O81" s="23"/>
@@ -2873,9 +2910,11 @@
       <c r="Q81" s="23"/>
       <c r="R81" s="24"/>
       <c r="S81" s="23"/>
-      <c r="T81" s="25"/>
-    </row>
-    <row r="82" spans="1:20">
+      <c r="T81" s="24"/>
+      <c r="U81" s="23"/>
+      <c r="V81" s="25"/>
+    </row>
+    <row r="82" spans="1:22">
       <c r="A82" s="7"/>
       <c r="B82" s="23"/>
       <c r="C82" s="28"/>
@@ -2886,8 +2925,6 @@
       <c r="H82" s="26"/>
       <c r="I82" s="24"/>
       <c r="J82" s="25"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="24"/>
       <c r="M82" s="23"/>
       <c r="N82" s="24"/>
       <c r="O82" s="23"/>
@@ -2895,60 +2932,62 @@
       <c r="Q82" s="23"/>
       <c r="R82" s="24"/>
       <c r="S82" s="23"/>
-      <c r="T82" s="25"/>
-    </row>
-    <row r="83" spans="1:20">
+      <c r="T82" s="24"/>
+      <c r="U82" s="23"/>
+      <c r="V82" s="25"/>
+    </row>
+    <row r="83" spans="1:22">
       <c r="C83" s="28"/>
       <c r="D83" s="28"/>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:22">
       <c r="C84" s="28"/>
       <c r="D84" s="28"/>
       <c r="H84" s="26"/>
       <c r="I84" s="24"/>
       <c r="J84" s="25"/>
     </row>
-    <row r="85" spans="1:20">
+    <row r="85" spans="1:22">
       <c r="C85" s="28"/>
       <c r="D85" s="28"/>
       <c r="H85" s="26"/>
       <c r="I85" s="24"/>
       <c r="J85" s="25"/>
     </row>
-    <row r="86" spans="1:20">
+    <row r="86" spans="1:22">
       <c r="C86" s="28"/>
       <c r="D86" s="28"/>
       <c r="H86" s="9"/>
     </row>
-    <row r="87" spans="1:20">
+    <row r="87" spans="1:22">
       <c r="H87" s="9"/>
     </row>
-    <row r="88" spans="1:20">
+    <row r="88" spans="1:22">
       <c r="H88" s="9"/>
     </row>
-    <row r="89" spans="1:20">
+    <row r="89" spans="1:22">
       <c r="H89" s="9"/>
     </row>
-    <row r="90" spans="1:20">
+    <row r="90" spans="1:22">
       <c r="H90" s="9"/>
     </row>
-    <row r="91" spans="1:20">
+    <row r="91" spans="1:22">
       <c r="H91" s="9"/>
     </row>
-    <row r="92" spans="1:20">
+    <row r="92" spans="1:22">
       <c r="H92" s="9"/>
     </row>
-    <row r="93" spans="1:20">
+    <row r="93" spans="1:22">
       <c r="H93" s="9"/>
     </row>
-    <row r="94" spans="1:20">
+    <row r="94" spans="1:22">
       <c r="H94" s="9"/>
     </row>
-    <row r="95" spans="1:20">
+    <row r="95" spans="1:22">
       <c r="H95" s="9"/>
     </row>
-    <row r="96" spans="1:20">
+    <row r="96" spans="1:22">
       <c r="H96" s="9"/>
     </row>
     <row r="97" spans="8:8">
@@ -6786,14 +6825,15 @@
       <c r="H1374" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="K1:T1"/>
+    <mergeCell ref="M1:V1"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -6821,7 +6861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -6840,34 +6880,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="21" customFormat="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="35"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:9" s="21" customFormat="1" ht="15" thickBot="1">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="36"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="19" t="s">
         <v>15</v>
       </c>

</xml_diff>